<commit_message>
updated legends for rolling corr and images
</commit_message>
<xml_diff>
--- a/reports/event_study/event_study_results.xlsx
+++ b/reports/event_study/event_study_results.xlsx
@@ -503,12 +503,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret corr</t>
+          <t>Alternative Strategy ret corr</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%) corr</t>
+          <t>Combined Portfolio ret (20.0%, levered) corr</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -584,7 +584,7 @@
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -615,7 +615,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2022-05 to 2022-05</t>
+          <t>2009-01 to 2009-07</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
@@ -624,89 +624,89 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.272362315750601</v>
+        <v>-0.01302304396289012</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1172247072326707</v>
+        <v>0.1294429039993541</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1070888447466593</v>
+        <v>0.07399579715559508</v>
       </c>
       <c r="F5" t="n">
-        <v>-2.323420737660782</v>
+        <v>-0.1006084038639546</v>
       </c>
       <c r="G5" t="n">
-        <v>-2.543330413125009</v>
+        <v>-0.1759970763678083</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.002376313140695137</v>
+        <v>-0.03401900207905247</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9748189366514745</v>
+        <v>0.9569526477258664</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.2496380921429677</v>
+        <v>0.09929037367779953</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1340081108899327</v>
+        <v>0.1944070382501609</v>
       </c>
       <c r="E6" t="n">
-        <v>0.08998020205555009</v>
+        <v>0.1218597218915814</v>
       </c>
       <c r="F6" t="n">
-        <v>-1.862858079896428</v>
+        <v>0.5107344598811989</v>
       </c>
       <c r="G6" t="n">
-        <v>-2.774366876714184</v>
+        <v>0.8147923869885259</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.002376313140695137</v>
+        <v>-0.03401900207905247</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2206807445260769</v>
+        <v>0.2575215155667883</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.3222899341791945</v>
+        <v>0.006835030772669744</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1201874663905772</v>
+        <v>0.1338835287369134</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1098054280362932</v>
+        <v>0.06921837659171393</v>
       </c>
       <c r="F7" t="n">
-        <v>-2.681560264627247</v>
+        <v>0.05105206620375879</v>
       </c>
       <c r="G7" t="n">
-        <v>-2.935100203540669</v>
+        <v>0.09874589826031777</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9748189366514745</v>
+        <v>0.9569526477258664</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2206807445260769</v>
+        <v>0.2575215155667883</v>
       </c>
       <c r="J7" t="n">
         <v>1</v>
@@ -715,7 +715,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2008-10 to 2008-12</t>
+          <t>2022-05 to 2022-07</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -724,89 +724,89 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.1367283582895165</v>
+        <v>-0.02961003418930468</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2857299553622801</v>
+        <v>0.1171029036386444</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1499964790942172</v>
+        <v>0.0848587164292048</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.4785230100083736</v>
+        <v>-0.2528548248528081</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.9115437849953361</v>
+        <v>-0.348933326301341</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.102994099951291</v>
+        <v>0.2850744758705622</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9825244972063308</v>
+        <v>0.9813052718846119</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.7839435180165524</v>
+        <v>-0.3592509127044985</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2668613361272396</v>
+        <v>0.1272259517147073</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2984087826954379</v>
+        <v>0.1248435402417852</v>
       </c>
       <c r="F9" t="n">
-        <v>-2.937643681896159</v>
+        <v>-2.823723523877316</v>
       </c>
       <c r="G9" t="n">
-        <v>-2.627079239878342</v>
+        <v>-2.87760914188059</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.102994099951291</v>
+        <v>0.2850744758705622</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.08394922944766235</v>
+        <v>0.4642168176218863</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.2935170618928271</v>
+        <v>-0.1014602167302045</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2852172414365627</v>
+        <v>0.1267257819783808</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1451962423697477</v>
+        <v>0.09293294100829544</v>
       </c>
       <c r="F10" t="n">
-        <v>-1.029099995548868</v>
+        <v>-0.8006280580498873</v>
       </c>
       <c r="G10" t="n">
-        <v>-2.021519683308159</v>
+        <v>-1.09175729971946</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9825244972063308</v>
+        <v>0.9813052718846119</v>
       </c>
       <c r="I10" t="n">
-        <v>0.08394922944766235</v>
+        <v>0.4642168176218863</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -815,7 +815,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>2022-05 to 2022-07</t>
+          <t>2022-05 to 2022-05</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
@@ -824,89 +824,89 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.02961003418930468</v>
+        <v>-0.272362315750601</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1171029036386444</v>
+        <v>0.1172247072326707</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0848587164292048</v>
+        <v>0.1070888447466593</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.2528548248528081</v>
+        <v>-2.323420737660782</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.348933326301341</v>
+        <v>-2.543330413125009</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2850744758705622</v>
+        <v>-0.002376313140695137</v>
       </c>
       <c r="J11" t="n">
-        <v>0.9813052718846119</v>
+        <v>0.9748189366514745</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.3592509127044985</v>
+        <v>-0.2496380921429677</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1272259517147073</v>
+        <v>0.1340081108899327</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1248435402417852</v>
+        <v>0.08998020205555009</v>
       </c>
       <c r="F12" t="n">
-        <v>-2.823723523877316</v>
+        <v>-1.862858079896428</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.87760914188059</v>
+        <v>-2.774366876714184</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2850744758705622</v>
+        <v>-0.002376313140695137</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0.4642168176218863</v>
+        <v>0.2206807445260769</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.1014602167302045</v>
+        <v>-0.3222899341791945</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1267257819783808</v>
+        <v>0.1201874663905772</v>
       </c>
       <c r="E13" t="n">
-        <v>0.09293294100829544</v>
+        <v>0.1098054280362932</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.8006280580498873</v>
+        <v>-2.681560264627247</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.09175729971946</v>
+        <v>-2.935100203540669</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9813052718846119</v>
+        <v>0.9748189366514745</v>
       </c>
       <c r="I13" t="n">
-        <v>0.4642168176218863</v>
+        <v>0.2206807445260769</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
@@ -915,7 +915,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>2022-08 to 2023-06</t>
+          <t>2008-10 to 2008-12</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
@@ -924,89 +924,89 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.000680760325932911</v>
+        <v>-0.1367283582895165</v>
       </c>
       <c r="D14" t="n">
-        <v>0.09684382864892992</v>
+        <v>0.2857299553622801</v>
       </c>
       <c r="E14" t="n">
-        <v>0.05672318903245911</v>
+        <v>0.1499964790942172</v>
       </c>
       <c r="F14" t="n">
-        <v>0.007029465226955719</v>
+        <v>-0.4785230100083736</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0120014466313478</v>
+        <v>-0.9115437849953361</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>0.09844291154644345</v>
+        <v>-0.102994099951291</v>
       </c>
       <c r="J14" t="n">
-        <v>0.978000487669424</v>
+        <v>0.9825244972063308</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.05692384517383346</v>
+        <v>-0.7839435180165524</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1060226998297278</v>
+        <v>0.2668613361272396</v>
       </c>
       <c r="E15" t="n">
-        <v>0.091892653538985</v>
+        <v>0.2984087826954379</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5369024300008681</v>
+        <v>-2.937643681896159</v>
       </c>
       <c r="G15" t="n">
-        <v>0.6194602395466118</v>
+        <v>-2.627079239878342</v>
       </c>
       <c r="H15" t="n">
-        <v>0.09844291154644345</v>
+        <v>-0.102994099951291</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3038665733897353</v>
+        <v>0.08394922944766235</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.01206552936069961</v>
+        <v>-0.2935170618928271</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1011566625461852</v>
+        <v>0.2852172414365627</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05928658783270815</v>
+        <v>0.1451962423697477</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1192756765298661</v>
+        <v>-1.029099995548868</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2035119544195308</v>
+        <v>-2.021519683308159</v>
       </c>
       <c r="H16" t="n">
-        <v>0.978000487669424</v>
+        <v>0.9825244972063308</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3038665733897353</v>
+        <v>0.08394922944766235</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
@@ -1015,7 +1015,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>2009-01 to 2009-07</t>
+          <t>1987-11 to 1987-12</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
@@ -1024,89 +1024,89 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.01302304396289012</v>
+        <v>-0.05625222242625717</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1294429039993541</v>
+        <v>0.1139220739009362</v>
       </c>
       <c r="E17" t="n">
-        <v>0.07399579715559508</v>
+        <v>0.06743173327094044</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.1006084038639546</v>
+        <v>-0.4937780756622524</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.1759970763678083</v>
+        <v>-0.8342099438588648</v>
       </c>
       <c r="H17" t="n">
         <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.03401900207905247</v>
+        <v>-0.327030465737847</v>
       </c>
       <c r="J17" t="n">
-        <v>0.9569526477258664</v>
+        <v>0.9494351755605979</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.09929037367779953</v>
+        <v>0.7060654565163512</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1944070382501609</v>
+        <v>0.1788536731317711</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1218597218915814</v>
+        <v>0.1756948713157408</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5107344598811989</v>
+        <v>3.947726899610024</v>
       </c>
       <c r="G18" t="n">
-        <v>0.8147923869885259</v>
+        <v>4.018702715843554</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.03401900207905247</v>
+        <v>-0.327030465737847</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2575215155667883</v>
+        <v>-0.01379473777596251</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.006835030772669744</v>
+        <v>0.08496086887701307</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1338835287369134</v>
+        <v>0.1076681763301386</v>
       </c>
       <c r="E19" t="n">
-        <v>0.06921837659171393</v>
+        <v>0.06306118749824347</v>
       </c>
       <c r="F19" t="n">
-        <v>0.05105206620375879</v>
+        <v>0.7890991727815742</v>
       </c>
       <c r="G19" t="n">
-        <v>0.09874589826031777</v>
+        <v>1.347276704540009</v>
       </c>
       <c r="H19" t="n">
-        <v>0.9569526477258664</v>
+        <v>0.9494351755605979</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2575215155667883</v>
+        <v>-0.01379473777596251</v>
       </c>
       <c r="J19" t="n">
         <v>1</v>
@@ -1115,7 +1115,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>1987-11 to 1987-12</t>
+          <t>2022-08 to 2023-06</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
@@ -1124,89 +1124,89 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.05625222242625717</v>
+        <v>0.000680760325932911</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1139220739009362</v>
+        <v>0.09684382864892992</v>
       </c>
       <c r="E20" t="n">
-        <v>0.06743173327094044</v>
+        <v>0.05672318903245911</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.4937780756622524</v>
+        <v>0.007029465226955719</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.8342099438588648</v>
+        <v>0.0120014466313478</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.327030465737847</v>
+        <v>0.09844291154644345</v>
       </c>
       <c r="J20" t="n">
-        <v>0.9494351755605979</v>
+        <v>0.978000487669424</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.7060654565163512</v>
+        <v>0.05692384517383346</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1788536731317711</v>
+        <v>0.1060226998297278</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1756948713157408</v>
+        <v>0.091892653538985</v>
       </c>
       <c r="F21" t="n">
-        <v>3.947726899610024</v>
+        <v>0.5369024300008681</v>
       </c>
       <c r="G21" t="n">
-        <v>4.018702715843554</v>
+        <v>0.6194602395466118</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.327030465737847</v>
+        <v>0.09844291154644345</v>
       </c>
       <c r="I21" t="n">
         <v>1</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.01379473777596251</v>
+        <v>0.3038665733897353</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.08496086887701307</v>
+        <v>0.01206552936069961</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1076681763301386</v>
+        <v>0.1011566625461852</v>
       </c>
       <c r="E22" t="n">
-        <v>0.06306118749824347</v>
+        <v>0.05928658783270815</v>
       </c>
       <c r="F22" t="n">
-        <v>0.7890991727815742</v>
+        <v>0.1192756765298661</v>
       </c>
       <c r="G22" t="n">
-        <v>1.347276704540009</v>
+        <v>0.2035119544195308</v>
       </c>
       <c r="H22" t="n">
-        <v>0.9494351755605979</v>
+        <v>0.978000487669424</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.01379473777596251</v>
+        <v>0.3038665733897353</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -1283,19 +1283,19 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret corr</t>
+          <t>Alternative Strategy ret corr</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%) corr</t>
+          <t>Combined Portfolio ret (20.0%, levered) corr</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Crimea Annexation</t>
+          <t>9-11 Attacks</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -1304,74 +1304,90 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0973821603652484</v>
+        <v>0.02326495911262535</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04149547350548922</v>
+        <v>0.08381872839702396</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02995209174529913</v>
+        <v>0.05181426850745924</v>
       </c>
       <c r="F2" t="n">
-        <v>2.346814053160912</v>
+        <v>0.2775627781231216</v>
       </c>
       <c r="G2" t="n">
-        <v>3.251264091781909</v>
+        <v>0.4490068041639168</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>-0.2644544857298831</v>
+      </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0.9331479970641047</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.1614721427983312</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+        <v>0.1514187555960346</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1007057381935775</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.066394596645066</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.603405582390429</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-0.2644544857298831</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.09991867815284498</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0973821603652484</v>
+        <v>0.05555938767229157</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04149547350548922</v>
+        <v>0.08124119090148399</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02995209174529913</v>
+        <v>0.05169276321004709</v>
       </c>
       <c r="F4" t="n">
-        <v>2.346814053160912</v>
+        <v>0.6838819945372896</v>
       </c>
       <c r="G4" t="n">
-        <v>3.251264091781909</v>
+        <v>1.074800111700993</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="inlineStr"/>
+        <v>0.9331479970641047</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.09991867815284498</v>
+      </c>
       <c r="J4" t="n">
         <v>1</v>
       </c>
@@ -1379,7 +1395,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Ukraine Invasion</t>
+          <t>Lebanon War</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
@@ -1388,89 +1404,89 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.03402450637303499</v>
+        <v>0.1612433234089805</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0842265164676608</v>
+        <v>0.04399451904588437</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05766520062785329</v>
+        <v>0.02189656943013704</v>
       </c>
       <c r="F5" t="n">
-        <v>0.403964307203645</v>
+        <v>3.665077534790429</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5900353419840626</v>
+        <v>7.363862358596477</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1666978448641719</v>
+        <v>0.08194788078356073</v>
       </c>
       <c r="J5" t="n">
-        <v>0.962797714014322</v>
+        <v>0.7399703549364588</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.119557900656519</v>
+        <v>0.004705427450738083</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1258456444096827</v>
+        <v>0.2168389350335898</v>
       </c>
       <c r="E6" t="n">
-        <v>0.09391021898985842</v>
+        <v>0.1514464585578704</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9500360637616162</v>
+        <v>0.02170010404270424</v>
       </c>
       <c r="G6" t="n">
-        <v>1.273108527938054</v>
+        <v>0.03106990744811676</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1666978448641719</v>
+        <v>0.08194788078356073</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4269385190774089</v>
+        <v>0.7310161405139033</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.05793608650433877</v>
+        <v>0.1621844088991281</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09183876812577579</v>
+        <v>0.0642571921539218</v>
       </c>
       <c r="E7" t="n">
-        <v>0.06217554058221185</v>
+        <v>0.03681722376878511</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6308456405359625</v>
+        <v>2.523988420014234</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9318147612682603</v>
+        <v>4.405123262896143</v>
       </c>
       <c r="H7" t="n">
-        <v>0.962797714014322</v>
+        <v>0.7399703549364588</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4269385190774089</v>
+        <v>0.7310161405139033</v>
       </c>
       <c r="J7" t="n">
         <v>1</v>
@@ -1479,7 +1495,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Invasion of Kuwait</t>
+          <t>Iraq War</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -1488,89 +1504,89 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.09764402904975139</v>
+        <v>0.08326972026968264</v>
       </c>
       <c r="D8" t="n">
-        <v>0.08305260930357274</v>
+        <v>0.0727019038983929</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04590779317156534</v>
+        <v>0.04143124334668843</v>
       </c>
       <c r="F8" t="n">
-        <v>1.175688878032047</v>
+        <v>1.145358179148364</v>
       </c>
       <c r="G8" t="n">
-        <v>2.126959766609534</v>
+        <v>2.009829142053453</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.1311252695892482</v>
+        <v>-0.4225986295490997</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9527623306810872</v>
+        <v>0.8570847414573305</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.1652704947595924</v>
+        <v>-0.03532594946237712</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1281261664912371</v>
+        <v>0.1883063268819927</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2498780065338474</v>
+        <v>0.1324406633638782</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.289904312956212</v>
+        <v>-0.1875983141262964</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.661404727259202</v>
+        <v>-0.2667303875194262</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1311252695892482</v>
+        <v>-0.4225986295490997</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1761633092331191</v>
+        <v>0.1047094024671635</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0645899300978329</v>
+        <v>0.0762045303772072</v>
       </c>
       <c r="D10" t="n">
-        <v>0.08364362350690764</v>
+        <v>0.06625518109992978</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04967767373649238</v>
+        <v>0.040917610997956</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7722038738852435</v>
+        <v>1.150167113154083</v>
       </c>
       <c r="G10" t="n">
-        <v>1.300180246773235</v>
+        <v>1.862389531515267</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9527623306810872</v>
+        <v>0.8570847414573305</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1761633092331191</v>
+        <v>0.1047094024671635</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -1579,7 +1595,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>9-11 Attacks</t>
+          <t>Apartheid Sanctions</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
@@ -1588,89 +1604,89 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.02326495911262535</v>
+        <v>0.03763902356687632</v>
       </c>
       <c r="D11" t="n">
-        <v>0.08381872839702396</v>
+        <v>0.108058981899841</v>
       </c>
       <c r="E11" t="n">
-        <v>0.05181426850745924</v>
+        <v>0.106195281236305</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2775627781231216</v>
+        <v>0.3483192503309316</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4490068041639168</v>
+        <v>0.3544321661818685</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.2644544857298831</v>
+        <v>-0.1609358549170533</v>
       </c>
       <c r="J11" t="n">
-        <v>0.9331479970641047</v>
+        <v>0.9556528318132864</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1614721427983312</v>
+        <v>0.07401037885776107</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1514187555960346</v>
+        <v>0.1606258607271223</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1007057381935775</v>
+        <v>0.1215343377215573</v>
       </c>
       <c r="F12" t="n">
-        <v>1.066394596645066</v>
+        <v>0.4607625355140845</v>
       </c>
       <c r="G12" t="n">
-        <v>1.603405582390429</v>
+        <v>0.6089668174876092</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.2644544857298831</v>
+        <v>-0.1609358549170533</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0.09991867815284498</v>
+        <v>0.1368580165854978</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.05555938767229157</v>
+        <v>0.05244109933842853</v>
       </c>
       <c r="D13" t="n">
-        <v>0.08124119090148399</v>
+        <v>0.1076634593977343</v>
       </c>
       <c r="E13" t="n">
-        <v>0.05169276321004709</v>
+        <v>0.1005424548287931</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6838819945372896</v>
+        <v>0.4870835437741111</v>
       </c>
       <c r="G13" t="n">
-        <v>1.074800111700993</v>
+        <v>0.5215816485456509</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9331479970641047</v>
+        <v>0.9556528318132864</v>
       </c>
       <c r="I13" t="n">
-        <v>0.09991867815284498</v>
+        <v>0.1368580165854978</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
@@ -1679,7 +1695,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Iraq War</t>
+          <t>Ukraine Invasion</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
@@ -1688,89 +1704,89 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.08326972026968264</v>
+        <v>0.03402450637303499</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0727019038983929</v>
+        <v>0.0842265164676608</v>
       </c>
       <c r="E14" t="n">
-        <v>0.04143124334668843</v>
+        <v>0.05766520062785329</v>
       </c>
       <c r="F14" t="n">
-        <v>1.145358179148364</v>
+        <v>0.403964307203645</v>
       </c>
       <c r="G14" t="n">
-        <v>2.009829142053453</v>
+        <v>0.5900353419840626</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.4225986295490997</v>
+        <v>0.1666978448641719</v>
       </c>
       <c r="J14" t="n">
-        <v>0.8570847414573305</v>
+        <v>0.962797714014322</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.03532594946237712</v>
+        <v>0.119557900656519</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1883063268819927</v>
+        <v>0.1258456444096827</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1324406633638782</v>
+        <v>0.09391021898985842</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.1875983141262964</v>
+        <v>0.9500360637616162</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.2667303875194262</v>
+        <v>1.273108527938054</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.4225986295490997</v>
+        <v>0.1666978448641719</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1047094024671635</v>
+        <v>0.4269385190774089</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.0762045303772072</v>
+        <v>0.05793608650433877</v>
       </c>
       <c r="D16" t="n">
-        <v>0.06625518109992978</v>
+        <v>0.09183876812577579</v>
       </c>
       <c r="E16" t="n">
-        <v>0.040917610997956</v>
+        <v>0.06217554058221185</v>
       </c>
       <c r="F16" t="n">
-        <v>1.150167113154083</v>
+        <v>0.6308456405359625</v>
       </c>
       <c r="G16" t="n">
-        <v>1.862389531515267</v>
+        <v>0.9318147612682603</v>
       </c>
       <c r="H16" t="n">
-        <v>0.8570847414573305</v>
+        <v>0.962797714014322</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1047094024671635</v>
+        <v>0.4269385190774089</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
@@ -1779,7 +1795,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Lehman Bankruptcy</t>
+          <t>Crimea Annexation</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
@@ -1788,90 +1804,74 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.05264490548546251</v>
+        <v>0.0973821603652484</v>
       </c>
       <c r="D17" t="n">
-        <v>0.139255861640943</v>
+        <v>0.04149547350548922</v>
       </c>
       <c r="E17" t="n">
-        <v>0.09800955160892749</v>
+        <v>0.02995209174529913</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.3780444490099958</v>
+        <v>2.346814053160912</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.5371405604988727</v>
+        <v>3.251264091781909</v>
       </c>
       <c r="H17" t="n">
         <v>1</v>
       </c>
-      <c r="I17" t="n">
-        <v>-0.1446932659830807</v>
-      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="n">
-        <v>0.9388890810019558</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.007107505281802848</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2448605103765675</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.1815391878339568</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.02902675188772709</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.03915135550955347</v>
-      </c>
-      <c r="H18" t="n">
-        <v>-0.1446932659830807</v>
-      </c>
-      <c r="I18" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.204746528225092</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.05122340442910193</v>
+        <v>0.0973821603652484</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1407726758400057</v>
+        <v>0.04149547350548922</v>
       </c>
       <c r="E19" t="n">
-        <v>0.09759666880724292</v>
+        <v>0.02995209174529913</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.3638732028317738</v>
+        <v>2.346814053160912</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.5248478770343081</v>
+        <v>3.251264091781909</v>
       </c>
       <c r="H19" t="n">
-        <v>0.9388890810019558</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.204746528225092</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="n">
         <v>1</v>
       </c>
@@ -1879,7 +1879,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Apartheid Sanctions</t>
+          <t>Invasion of Kuwait</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
@@ -1888,89 +1888,89 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.03763902356687632</v>
+        <v>0.09764402904975139</v>
       </c>
       <c r="D20" t="n">
-        <v>0.108058981899841</v>
+        <v>0.08305260930357274</v>
       </c>
       <c r="E20" t="n">
-        <v>0.106195281236305</v>
+        <v>0.04590779317156534</v>
       </c>
       <c r="F20" t="n">
-        <v>0.3483192503309316</v>
+        <v>1.175688878032047</v>
       </c>
       <c r="G20" t="n">
-        <v>0.3544321661818685</v>
+        <v>2.126959766609534</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.1609358549170533</v>
+        <v>-0.1311252695892482</v>
       </c>
       <c r="J20" t="n">
-        <v>0.9556528318132864</v>
+        <v>0.9527623306810872</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.07401037885776107</v>
+        <v>-0.1652704947595924</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1606258607271223</v>
+        <v>0.1281261664912371</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1215343377215573</v>
+        <v>0.2498780065338474</v>
       </c>
       <c r="F21" t="n">
-        <v>0.4607625355140845</v>
+        <v>-1.289904312956212</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6089668174876092</v>
+        <v>-0.661404727259202</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.1609358549170533</v>
+        <v>-0.1311252695892482</v>
       </c>
       <c r="I21" t="n">
         <v>1</v>
       </c>
       <c r="J21" t="n">
-        <v>0.1368580165854978</v>
+        <v>0.1761633092331191</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.05244109933842853</v>
+        <v>0.0645899300978329</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1076634593977343</v>
+        <v>0.08364362350690764</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1005424548287931</v>
+        <v>0.04967767373649238</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4870835437741111</v>
+        <v>0.7722038738852435</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5215816485456509</v>
+        <v>1.300180246773235</v>
       </c>
       <c r="H22" t="n">
-        <v>0.9556528318132864</v>
+        <v>0.9527623306810872</v>
       </c>
       <c r="I22" t="n">
-        <v>0.1368580165854978</v>
+        <v>0.1761633092331191</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -1979,7 +1979,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Lebanon War</t>
+          <t>Lehman Bankruptcy</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
@@ -1988,89 +1988,89 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.1612433234089805</v>
+        <v>-0.05264490548546251</v>
       </c>
       <c r="D23" t="n">
-        <v>0.04399451904588437</v>
+        <v>0.139255861640943</v>
       </c>
       <c r="E23" t="n">
-        <v>0.02189656943013704</v>
+        <v>0.09800955160892749</v>
       </c>
       <c r="F23" t="n">
-        <v>3.665077534790429</v>
+        <v>-0.3780444490099958</v>
       </c>
       <c r="G23" t="n">
-        <v>7.363862358596477</v>
+        <v>-0.5371405604988727</v>
       </c>
       <c r="H23" t="n">
         <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>0.08194788078356073</v>
+        <v>-0.1446932659830807</v>
       </c>
       <c r="J23" t="n">
-        <v>0.7399703549364588</v>
+        <v>0.9388890810019558</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Strategy ret</t>
+          <t>Alternative Strategy ret</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.004705427450738083</v>
+        <v>0.007107505281802848</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2168389350335898</v>
+        <v>0.2448605103765675</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1514464585578704</v>
+        <v>0.1815391878339568</v>
       </c>
       <c r="F24" t="n">
-        <v>0.02170010404270424</v>
+        <v>0.02902675188772709</v>
       </c>
       <c r="G24" t="n">
-        <v>0.03106990744811676</v>
+        <v>0.03915135550955347</v>
       </c>
       <c r="H24" t="n">
-        <v>0.08194788078356073</v>
+        <v>-0.1446932659830807</v>
       </c>
       <c r="I24" t="n">
         <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>0.7310161405139033</v>
+        <v>0.204746528225092</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Combined (100% / 20.0%)</t>
+          <t>Combined Portfolio ret (20.0%, levered)</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.1621844088991281</v>
+        <v>-0.05122340442910193</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0642571921539218</v>
+        <v>0.1407726758400057</v>
       </c>
       <c r="E25" t="n">
-        <v>0.03681722376878511</v>
+        <v>0.09759666880724292</v>
       </c>
       <c r="F25" t="n">
-        <v>2.523988420014234</v>
+        <v>-0.3638732028317738</v>
       </c>
       <c r="G25" t="n">
-        <v>4.405123262896143</v>
+        <v>-0.5248478770343081</v>
       </c>
       <c r="H25" t="n">
-        <v>0.7399703549364588</v>
+        <v>0.9388890810019558</v>
       </c>
       <c r="I25" t="n">
-        <v>0.7310161405139033</v>
+        <v>0.204746528225092</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>

</xml_diff>